<commit_message>
add measures to file
</commit_message>
<xml_diff>
--- a/pomiary grain grow.xlsx
+++ b/pomiary grain grow.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>rozmiar danych</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>weak scalability - zwiekszamy przestrzen proporcjonalnie do ilosci prockow</t>
+  </si>
+  <si>
+    <t>space/cores</t>
+  </si>
+  <si>
+    <t>number of tasks for one core:</t>
+  </si>
+  <si>
+    <t>Busy Leafs algorithm</t>
+  </si>
+  <si>
+    <t>F0035595649/007/15</t>
   </si>
 </sst>
 </file>
@@ -410,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M13"/>
+  <dimension ref="A2:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,9 +434,10 @@
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>4</v>
       </c>
@@ -450,7 +463,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -464,7 +477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -484,7 +497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -504,7 +517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -517,8 +530,14 @@
       <c r="D6">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -531,8 +550,35 @@
       <c r="D7">
         <v>208</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>20</v>
+      </c>
+      <c r="O7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -545,8 +591,32 @@
       <c r="D8">
         <v>358</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>162</v>
+      </c>
+      <c r="J8">
+        <v>417</v>
+      </c>
+      <c r="K8">
+        <v>900</v>
+      </c>
+      <c r="L8">
+        <v>1359</v>
+      </c>
+      <c r="M8">
+        <v>2545</v>
+      </c>
+      <c r="N8">
+        <v>2359</v>
+      </c>
+      <c r="O8">
+        <v>3479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -559,8 +629,32 @@
       <c r="D9">
         <v>1653</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>764</v>
+      </c>
+      <c r="J9">
+        <v>647</v>
+      </c>
+      <c r="K9">
+        <v>1019</v>
+      </c>
+      <c r="L9">
+        <v>1396</v>
+      </c>
+      <c r="M9">
+        <v>1493</v>
+      </c>
+      <c r="N9">
+        <v>2440</v>
+      </c>
+      <c r="O9">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -573,8 +667,32 @@
       <c r="D10">
         <v>3016</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>2736</v>
+      </c>
+      <c r="J10">
+        <v>1146</v>
+      </c>
+      <c r="K10">
+        <v>1260</v>
+      </c>
+      <c r="L10">
+        <v>1521</v>
+      </c>
+      <c r="M10">
+        <v>1808</v>
+      </c>
+      <c r="N10">
+        <v>2308</v>
+      </c>
+      <c r="O10">
+        <v>2738</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -587,10 +705,882 @@
       <c r="D11">
         <v>5943</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>14164</v>
+      </c>
+      <c r="J11">
+        <v>4984</v>
+      </c>
+      <c r="K11">
+        <v>2561</v>
+      </c>
+      <c r="L11">
+        <v>2131</v>
+      </c>
+      <c r="M11">
+        <v>2405</v>
+      </c>
+      <c r="N11">
+        <v>2698</v>
+      </c>
+      <c r="O11">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>68153</v>
+      </c>
+      <c r="J12">
+        <v>22197</v>
+      </c>
+      <c r="K12">
+        <v>10106</v>
+      </c>
+      <c r="L12">
+        <v>6903</v>
+      </c>
+      <c r="M12">
+        <v>6831</v>
+      </c>
+      <c r="N12">
+        <v>7070</v>
+      </c>
+      <c r="O12">
+        <v>7299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>432309</v>
+      </c>
+      <c r="J13">
+        <v>147447</v>
+      </c>
+      <c r="K13">
+        <v>65538</v>
+      </c>
+      <c r="L13">
+        <v>43053</v>
+      </c>
+      <c r="M13">
+        <v>41181</v>
+      </c>
+      <c r="N13">
+        <v>40775</v>
+      </c>
+      <c r="O13">
+        <v>40871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>850560</v>
+      </c>
+      <c r="J14">
+        <v>291565</v>
+      </c>
+      <c r="K14">
+        <v>129057</v>
+      </c>
+      <c r="L14">
+        <v>84767</v>
+      </c>
+      <c r="M14">
+        <v>80167</v>
+      </c>
+      <c r="N14">
+        <v>79690</v>
+      </c>
+      <c r="O14">
+        <v>78969</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>1785336</v>
+      </c>
+      <c r="J15">
+        <v>598514</v>
+      </c>
+      <c r="K15">
+        <v>263654</v>
+      </c>
+      <c r="L15">
+        <v>177483</v>
+      </c>
+      <c r="M15">
+        <v>166947</v>
+      </c>
+      <c r="N15">
+        <v>163891</v>
+      </c>
+      <c r="O15">
+        <v>160834</v>
+      </c>
+    </row>
+    <row r="18" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>12</v>
+      </c>
+      <c r="M19">
+        <v>16</v>
+      </c>
+      <c r="N19">
+        <v>20</v>
+      </c>
+      <c r="O19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>123</v>
+      </c>
+      <c r="J20">
+        <v>239</v>
+      </c>
+      <c r="K20">
+        <v>500</v>
+      </c>
+      <c r="L20">
+        <v>779</v>
+      </c>
+      <c r="M20">
+        <v>1821</v>
+      </c>
+      <c r="N20">
+        <v>1250</v>
+      </c>
+      <c r="O20">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="21" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>1023</v>
+      </c>
+      <c r="J21">
+        <v>399</v>
+      </c>
+      <c r="K21">
+        <v>578</v>
+      </c>
+      <c r="L21">
+        <v>837</v>
+      </c>
+      <c r="M21">
+        <v>825</v>
+      </c>
+      <c r="N21">
+        <v>1367</v>
+      </c>
+      <c r="O21">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="22" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>2662</v>
+      </c>
+      <c r="J22">
+        <v>1062</v>
+      </c>
+      <c r="K22">
+        <v>969</v>
+      </c>
+      <c r="L22">
+        <v>879</v>
+      </c>
+      <c r="M22">
+        <v>1176</v>
+      </c>
+      <c r="N22">
+        <v>1572</v>
+      </c>
+      <c r="O22">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="23" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>13878</v>
+      </c>
+      <c r="J23">
+        <v>4851</v>
+      </c>
+      <c r="K23">
+        <v>2349</v>
+      </c>
+      <c r="L23">
+        <v>1766</v>
+      </c>
+      <c r="M23">
+        <v>1835</v>
+      </c>
+      <c r="N23">
+        <v>2301</v>
+      </c>
+      <c r="O23">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="24" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>65147</v>
+      </c>
+      <c r="J24">
+        <v>22044</v>
+      </c>
+      <c r="K24">
+        <v>9897</v>
+      </c>
+      <c r="L24">
+        <v>6611</v>
+      </c>
+      <c r="M24">
+        <v>6338</v>
+      </c>
+      <c r="N24">
+        <v>6411</v>
+      </c>
+      <c r="O24">
+        <v>6569</v>
+      </c>
+    </row>
+    <row r="25" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>429074</v>
+      </c>
+      <c r="J25">
+        <v>147013</v>
+      </c>
+      <c r="K25">
+        <v>67017</v>
+      </c>
+      <c r="L25">
+        <v>44021</v>
+      </c>
+      <c r="M25">
+        <v>40656</v>
+      </c>
+      <c r="N25">
+        <v>40283</v>
+      </c>
+      <c r="O25">
+        <v>40040</v>
+      </c>
+    </row>
+    <row r="26" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26">
+        <v>846530</v>
+      </c>
+      <c r="J26">
+        <v>289460</v>
+      </c>
+      <c r="K26">
+        <v>128455</v>
+      </c>
+      <c r="L26">
+        <v>85767</v>
+      </c>
+      <c r="M26">
+        <v>80702</v>
+      </c>
+      <c r="N26">
+        <v>79270</v>
+      </c>
+      <c r="O26">
+        <v>78468</v>
+      </c>
+    </row>
+    <row r="27" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <v>1784510</v>
+      </c>
+      <c r="J27">
+        <v>597497</v>
+      </c>
+      <c r="K27">
+        <v>264576</v>
+      </c>
+      <c r="L27">
+        <v>178132</v>
+      </c>
+      <c r="M27">
+        <v>166023</v>
+      </c>
+      <c r="N27">
+        <v>164377</v>
+      </c>
+      <c r="O27">
+        <v>161849</v>
+      </c>
+    </row>
+    <row r="31" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>8</v>
+      </c>
+      <c r="L33">
+        <v>12</v>
+      </c>
+      <c r="M33">
+        <v>16</v>
+      </c>
+      <c r="N33">
+        <v>20</v>
+      </c>
+      <c r="O33">
+        <v>24</v>
+      </c>
+      <c r="R33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>206</v>
+      </c>
+      <c r="J34">
+        <v>2262</v>
+      </c>
+      <c r="K34">
+        <v>9513</v>
+      </c>
+      <c r="L34">
+        <v>16369</v>
+      </c>
+      <c r="M34">
+        <v>24049</v>
+      </c>
+      <c r="N34">
+        <v>28789</v>
+      </c>
+      <c r="O34">
+        <v>36266</v>
+      </c>
+      <c r="R34">
+        <v>112.17</v>
+      </c>
+    </row>
+    <row r="35" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35">
+        <v>777</v>
+      </c>
+      <c r="J35">
+        <v>1563</v>
+      </c>
+      <c r="K35">
+        <v>9547</v>
+      </c>
+      <c r="L35">
+        <v>16632</v>
+      </c>
+      <c r="M35">
+        <v>21509</v>
+      </c>
+      <c r="N35">
+        <v>28829</v>
+      </c>
+      <c r="O35">
+        <v>35108</v>
+      </c>
+    </row>
+    <row r="36" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>2758</v>
+      </c>
+      <c r="J36">
+        <v>2583</v>
+      </c>
+      <c r="K36">
+        <v>8406</v>
+      </c>
+      <c r="L36">
+        <v>16501</v>
+      </c>
+      <c r="M36">
+        <v>23053</v>
+      </c>
+      <c r="N36">
+        <v>29359</v>
+      </c>
+      <c r="O36">
+        <v>35643</v>
+      </c>
+    </row>
+    <row r="37" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37">
+        <v>14168</v>
+      </c>
+      <c r="J37">
+        <v>6261</v>
+      </c>
+      <c r="K37">
+        <v>7874</v>
+      </c>
+      <c r="L37">
+        <v>14300</v>
+      </c>
+      <c r="M37">
+        <v>23031</v>
+      </c>
+      <c r="N37">
+        <v>29512</v>
+      </c>
+      <c r="O37">
+        <v>35484</v>
+      </c>
+    </row>
+    <row r="38" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38">
+        <v>66303</v>
+      </c>
+      <c r="J38">
+        <v>24437</v>
+      </c>
+      <c r="K38">
+        <v>12025</v>
+      </c>
+      <c r="L38">
+        <v>13889</v>
+      </c>
+      <c r="M38">
+        <v>18478</v>
+      </c>
+      <c r="N38">
+        <v>25076</v>
+      </c>
+      <c r="O38">
+        <v>35809</v>
+      </c>
+    </row>
+    <row r="39" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>430033</v>
+      </c>
+      <c r="J39">
+        <v>153180</v>
+      </c>
+      <c r="K39">
+        <v>69547</v>
+      </c>
+      <c r="L39">
+        <v>45050</v>
+      </c>
+      <c r="M39">
+        <v>42698</v>
+      </c>
+      <c r="N39">
+        <v>47994</v>
+      </c>
+      <c r="O39">
+        <v>53750</v>
+      </c>
+    </row>
+    <row r="40" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40">
+        <v>849909</v>
+      </c>
+      <c r="J40">
+        <v>300651</v>
+      </c>
+      <c r="K40">
+        <v>135539</v>
+      </c>
+      <c r="L40">
+        <v>88898</v>
+      </c>
+      <c r="M40">
+        <v>82054</v>
+      </c>
+      <c r="N40">
+        <v>81591</v>
+      </c>
+      <c r="O40">
+        <v>84156</v>
+      </c>
+    </row>
+    <row r="41" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41">
+        <v>1747496</v>
+      </c>
+      <c r="J41">
+        <v>610503</v>
+      </c>
+      <c r="K41">
+        <v>274415</v>
+      </c>
+      <c r="L41">
+        <v>180236</v>
+      </c>
+      <c r="M41">
+        <v>166545</v>
+      </c>
+      <c r="N41">
+        <v>164711</v>
+      </c>
+      <c r="O41">
+        <v>161991</v>
+      </c>
+    </row>
+    <row r="45" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+      <c r="K46">
+        <v>8</v>
+      </c>
+      <c r="L46">
+        <v>12</v>
+      </c>
+      <c r="M46">
+        <v>16</v>
+      </c>
+      <c r="N46">
+        <v>20</v>
+      </c>
+      <c r="O46">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>139</v>
+      </c>
+      <c r="J47">
+        <v>1160</v>
+      </c>
+      <c r="K47">
+        <v>4673</v>
+      </c>
+      <c r="L47">
+        <v>7921</v>
+      </c>
+      <c r="M47">
+        <v>11755</v>
+      </c>
+      <c r="N47">
+        <v>14171</v>
+      </c>
+      <c r="O47">
+        <v>18097</v>
+      </c>
+    </row>
+    <row r="48" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>741</v>
+      </c>
+      <c r="J48">
+        <v>894</v>
+      </c>
+      <c r="K48">
+        <v>4584</v>
+      </c>
+      <c r="L48">
+        <v>8141</v>
+      </c>
+      <c r="M48">
+        <v>10675</v>
+      </c>
+      <c r="N48">
+        <v>14675</v>
+      </c>
+      <c r="O48">
+        <v>18153</v>
+      </c>
+    </row>
+    <row r="49" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>6</v>
+      </c>
+      <c r="I49">
+        <v>2627</v>
+      </c>
+      <c r="J49">
+        <v>1498</v>
+      </c>
+      <c r="K49">
+        <v>4098</v>
+      </c>
+      <c r="L49">
+        <v>8045</v>
+      </c>
+      <c r="M49">
+        <v>11447</v>
+      </c>
+      <c r="N49">
+        <v>14851</v>
+      </c>
+      <c r="O49">
+        <v>18112</v>
+      </c>
+    </row>
+    <row r="50" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50">
+        <v>13883</v>
+      </c>
+      <c r="J50">
+        <v>5414</v>
+      </c>
+      <c r="K50">
+        <v>3661</v>
+      </c>
+      <c r="L50">
+        <v>7119</v>
+      </c>
+      <c r="M50">
+        <v>10227</v>
+      </c>
+      <c r="N50">
+        <v>14797</v>
+      </c>
+      <c r="O50">
+        <v>18295</v>
+      </c>
+    </row>
+    <row r="51" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51">
+        <v>64960</v>
+      </c>
+      <c r="J51">
+        <v>23305</v>
+      </c>
+      <c r="K51">
+        <v>10731</v>
+      </c>
+      <c r="L51">
+        <v>7932</v>
+      </c>
+      <c r="M51">
+        <v>11165</v>
+      </c>
+      <c r="N51">
+        <v>12658</v>
+      </c>
+      <c r="O51">
+        <v>14487</v>
+      </c>
+    </row>
+    <row r="52" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52">
+        <v>425661</v>
+      </c>
+      <c r="J52">
+        <v>150156</v>
+      </c>
+      <c r="K52">
+        <v>67674</v>
+      </c>
+      <c r="L52">
+        <v>44429</v>
+      </c>
+      <c r="M52">
+        <v>40956</v>
+      </c>
+      <c r="N52">
+        <v>40813</v>
+      </c>
+      <c r="O52">
+        <v>42314</v>
+      </c>
+    </row>
+    <row r="53" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="I53">
+        <v>881189</v>
+      </c>
+      <c r="J53">
+        <v>295335</v>
+      </c>
+      <c r="K53">
+        <v>133116</v>
+      </c>
+      <c r="L53">
+        <v>86753</v>
+      </c>
+      <c r="M53">
+        <v>80951</v>
+      </c>
+      <c r="N53">
+        <v>79601</v>
+      </c>
+      <c r="O53">
+        <v>79056</v>
+      </c>
+    </row>
+    <row r="54" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54">
+        <v>1771224</v>
+      </c>
+      <c r="J54">
+        <v>596272</v>
+      </c>
+      <c r="K54">
+        <v>268239</v>
+      </c>
+      <c r="L54">
+        <v>174486</v>
+      </c>
+      <c r="M54">
+        <v>167737</v>
+      </c>
+      <c r="N54">
+        <v>162763</v>
+      </c>
+      <c r="O54">
+        <v>160425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new simple parallel  measures
</commit_message>
<xml_diff>
--- a/pomiary grain grow.xlsx
+++ b/pomiary grain grow.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>rozmiar danych</t>
   </si>
@@ -81,6 +81,15 @@
   <si>
     <t>6000x4000</t>
   </si>
+  <si>
+    <t>number of all taksk:</t>
+  </si>
+  <si>
+    <t>without work stealing algorithm: weak scalability</t>
+  </si>
+  <si>
+    <t>simple parallel algorithm</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -111,6 +120,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -241,10 +256,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart289.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Work stealing algorithm: weak scalability</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -255,11 +290,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$G$24</c:f>
+              <c:f>Arkusz1!$R$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7000x7000</c:v>
+                  <c:v>Work stealing algorithm: weak scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -276,37 +311,33 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="4"/>
           </c:marker>
-          <c:smooth val="1"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$H$7:$O$7</c:f>
+              <c:f>Arkusz1!$S$8:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -314,68 +345,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$H$24:$O$24</c:f>
+              <c:f>Arkusz1!$T$8:$T$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>275037</c:v>
+                  <c:v>5793</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>152714</c:v>
+                  <c:v>5963</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79585</c:v>
+                  <c:v>6018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39899</c:v>
+                  <c:v>6843</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34211</c:v>
+                  <c:v>8387</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32528</c:v>
+                  <c:v>10518</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30326</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>31088</c:v>
+                  <c:v>12334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56330032"/>
-        <c:axId val="75264000"/>
+        <c:axId val="74332220"/>
+        <c:axId val="30468655"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56330032"/>
+        <c:axId val="74332220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="75264000"/>
-        <c:crossesAt val="0"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="75264000"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln>
@@ -395,7 +403,45 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="56330032"/>
+        <c:crossAx val="30468655"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="30468655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="74332220"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -430,10 +476,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart290.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Work stealing algorithm: weak scalability</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -444,11 +510,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$G$13</c:f>
+              <c:f>Arkusz1!$R$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10000x10000</c:v>
+                  <c:v>Work stealing algorithm: weak scalability</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -465,37 +531,34 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$H$7:$O$7</c:f>
+              <c:f>Arkusz1!$S$20:$S$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -503,43 +566,40 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$H$13:$O$13</c:f>
+              <c:f>Arkusz1!$T$20:$T$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>565296</c:v>
+                  <c:v>5995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>312850</c:v>
+                  <c:v>6068</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>164028</c:v>
+                  <c:v>6133</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81061</c:v>
+                  <c:v>7054</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70184</c:v>
+                  <c:v>8551</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65339</c:v>
+                  <c:v>10602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61368</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>62512</c:v>
+                  <c:v>12371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87974457"/>
-        <c:axId val="46997240"/>
+        <c:axId val="74536273"/>
+        <c:axId val="41795194"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87974457"/>
+        <c:axId val="74536273"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -555,11 +615,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46997240"/>
+        <c:crossAx val="41795194"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46997240"/>
+        <c:axId val="41795194"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +644,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87974457"/>
+        <c:crossAx val="74536273"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -619,10 +679,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart291.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>500x500</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -633,11 +713,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$R$5</c:f>
+              <c:f>Arkusz1!$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Work stealing algorithm: weak scalability</c:v>
+                  <c:v>500x500</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -654,59 +734,37 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="4"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Arkusz1!$S$9:$S$14</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
+          <c:smooth val="1"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$S$8:$S$14</c:f>
+              <c:f>Arkusz1!$H$7:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
@@ -714,270 +772,43 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$T$8:$T$14</c:f>
+              <c:f>Arkusz1!$H$8:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5793</c:v>
+                  <c:v>1190</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5963</c:v>
+                  <c:v>843</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6018</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6843</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8387</c:v>
+                  <c:v>387</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10518</c:v>
+                  <c:v>317</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12334</c:v>
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>409</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="31167361"/>
-        <c:axId val="64239683"/>
+        <c:axId val="98177937"/>
+        <c:axId val="9500022"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="31167361"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="64239683"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="64239683"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="31167361"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$R$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Work stealing algorithm: weak scalability</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Arkusz1!$S$20:$S$26</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Arkusz1!$S$20:$S$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Arkusz1!$T$20:$T$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>5995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6068</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6133</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7054</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8551</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10602</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12371</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="77808810"/>
-        <c:axId val="85633375"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="77808810"/>
+        <c:axId val="98177937"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,11 +824,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="85633375"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="9500022"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85633375"/>
+        <c:axId val="9500022"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,574 +853,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77808810"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$G$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>500x500</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Arkusz1!$H$7:$O$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Arkusz1!$H$8:$O$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1190</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>843</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>570</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>387</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>317</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>409</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="19791764"/>
-        <c:axId val="11502198"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="19791764"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="11502198"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="11502198"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="19791764"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$G$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1000x1000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Arkusz1!$H$7:$O$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Arkusz1!$H$9:$O$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5204</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3223</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1630</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>769</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1102</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>890</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>631</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>974</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="67084523"/>
-        <c:axId val="98735105"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="67084523"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="98735105"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="98735105"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="67084523"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$G$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2000x2000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:size val="7"/>
-          </c:marker>
-          <c:smooth val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Arkusz1!$H$7:$O$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Arkusz1!$H$10:$O$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>22152</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12603</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6141</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3229</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3261</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2891</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2488</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2691</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="37262811"/>
-        <c:axId val="13323789"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="37262811"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="13323789"/>
-        <c:crossesAt val="0"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="13323789"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="37262811"/>
+        <c:crossAx val="98177937"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1624,10 +888,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart292.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>1000x1000</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1638,11 +922,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$G$11</c:f>
+              <c:f>Arkusz1!$G$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5000x5000</c:v>
+                  <c:v>1000x1000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1659,7 +943,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="4"/>
           </c:marker>
           <c:smooth val="1"/>
           <c:xVal>
@@ -1697,43 +981,43 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$H$11:$O$11</c:f>
+              <c:f>Arkusz1!$H$9:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>139995</c:v>
+                  <c:v>5204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77163</c:v>
+                  <c:v>3223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40463</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20601</c:v>
+                  <c:v>769</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18111</c:v>
+                  <c:v>1102</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16705</c:v>
+                  <c:v>890</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15965</c:v>
+                  <c:v>631</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16165</c:v>
+                  <c:v>974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="27957351"/>
-        <c:axId val="18259894"/>
+        <c:axId val="34442817"/>
+        <c:axId val="49067966"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27957351"/>
+        <c:axId val="34442817"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,11 +1033,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18259894"/>
+        <c:crossAx val="49067966"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18259894"/>
+        <c:axId val="49067966"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1062,843 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27957351"/>
+        <c:crossAx val="34442817"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart293.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2000x2000</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2000x2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="4"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$10:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>22152</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12603</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3229</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2488</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2691</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="49743948"/>
+        <c:axId val="57295647"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="49743948"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="57295647"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="57295647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="49743948"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart294.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>5000x5000</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$G$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5000x5000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="4"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$11:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>139995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40463</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16705</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15965</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16165</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="9518913"/>
+        <c:axId val="38182278"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="9518913"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="38182278"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="38182278"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="9518913"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart295.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>7000x7000</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$G$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7000x7000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="4"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$24:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>275037</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152714</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34211</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32528</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30326</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31088</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="86774831"/>
+        <c:axId val="190780"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="86774831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="190780"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="190780"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="86774831"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart296.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>10000x10000</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$G$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10000x10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="4"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$H$13:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>565296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>312850</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164028</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81061</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70184</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65339</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61368</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="27491494"/>
+        <c:axId val="42071282"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="27491494"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="42071282"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="42071282"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="27491494"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1818,15 +1938,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>57600</xdr:colOff>
+      <xdr:colOff>138600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>488880</xdr:colOff>
+      <xdr:colOff>568800</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>101520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1834,8 +1954,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="24609600" y="74880"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="24690600" y="47880"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1847,16 +1967,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>720360</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38880</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>394560</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:colOff>474480</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1864,8 +1984,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="24509880" y="3608640"/>
-        <a:ext cx="5765040" cy="3240360"/>
+        <a:off x="24590880" y="3581640"/>
+        <a:ext cx="5763960" cy="3422160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1878,15 +1998,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>700920</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:colOff>781920</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1540440</xdr:colOff>
+      <xdr:colOff>1620360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1894,8 +2014,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="700920" y="2134440"/>
-        <a:ext cx="5754960" cy="3240360"/>
+        <a:off x="781920" y="2107440"/>
+        <a:ext cx="5753880" cy="3300480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1907,16 +2027,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>785520</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>131040</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1628640</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1924,8 +2044,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1687680" y="5989320"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="785520" y="6127560"/>
+        <a:ext cx="5758560" cy="3512880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1937,16 +2057,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>25920</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>686160</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>16920</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1529280</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1954,8 +2074,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8104680" y="5801760"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="686160" y="10112040"/>
+        <a:ext cx="5758560" cy="3528000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1967,16 +2087,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>756720</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1599840</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1984,8 +2104,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1658880" y="9663120"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="756720" y="14513400"/>
+        <a:ext cx="5758560" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1997,16 +2117,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>25920</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>738360</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>16920</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1581480</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2014,8 +2134,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8104680" y="9663120"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="738360" y="18564120"/>
+        <a:ext cx="5758560" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2027,16 +2147,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>779040</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1622160</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2044,8 +2164,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1658880" y="13737960"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="779040" y="22689360"/>
+        <a:ext cx="5758560" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2063,10 +2183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:T26"/>
+  <dimension ref="A2:T58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G80" activeCellId="0" sqref="G80"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E31" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2730,6 +2850,704 @@
         <v>12371</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T30" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>1190</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>832</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>386</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>334</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>213</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>348</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>5204</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>3195</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>1432</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>726</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>572</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>544</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>553</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>525</v>
+      </c>
+      <c r="R32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="S32" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>22152</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>12464</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>5824</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>2966</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>2028</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="R33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="S33" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>139995</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>78400</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>37611</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>19094</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <v>13115</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>12941</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>12976</v>
+      </c>
+      <c r="R34" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S34" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>275037</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>150886</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>73367</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>37505</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>25693</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <v>25620</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>25550</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>25548</v>
+      </c>
+      <c r="R35" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S35" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>565296</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>304583</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>149058</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>77466</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>53278</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <v>52671</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>52304</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>52353</v>
+      </c>
+      <c r="R36" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R37" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="S37" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="T37" s="0" t="n">
+        <v>12390</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="O42" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>1190</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>688</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>355</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G44" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>5204</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>2917</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>1448</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>755</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <v>743</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <v>562</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>477</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>22152</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>11894</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>5951</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>3044</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <v>2122</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>2427</v>
+      </c>
+      <c r="N45" s="0" t="n">
+        <v>2157</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>139995</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>73679</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>37074</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>19281</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <v>13557</v>
+      </c>
+      <c r="M46" s="0" t="n">
+        <v>14876</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>13844</v>
+      </c>
+      <c r="O46" s="0" t="n">
+        <v>13367</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>275037</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>144247</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>72456</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>38372</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>26554</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <v>29354</v>
+      </c>
+      <c r="N47" s="0" t="n">
+        <v>27867</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <v>27448</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <v>565296</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>297507</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <v>149203</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>77708</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>54392</v>
+      </c>
+      <c r="M48" s="0" t="n">
+        <v>60571</v>
+      </c>
+      <c r="N48" s="0" t="n">
+        <v>56887</v>
+      </c>
+      <c r="O48" s="0" t="n">
+        <v>54891</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M52" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="N52" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="O52" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G53" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>1190</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>674</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>341</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="M53" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="N53" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="O53" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <v>5204</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>2803</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>1398</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>743</v>
+      </c>
+      <c r="L54" s="0" t="n">
+        <v>529</v>
+      </c>
+      <c r="M54" s="0" t="n">
+        <v>658</v>
+      </c>
+      <c r="N54" s="0" t="n">
+        <v>551</v>
+      </c>
+      <c r="O54" s="0" t="n">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G55" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <v>22152</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>11791</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>5827</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>3025</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <v>3125</v>
+      </c>
+      <c r="M55" s="0" t="n">
+        <v>2617</v>
+      </c>
+      <c r="N55" s="0" t="n">
+        <v>2152</v>
+      </c>
+      <c r="O55" s="0" t="n">
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <v>139995</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>73997</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>37197</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>19502</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <v>13426</v>
+      </c>
+      <c r="M56" s="0" t="n">
+        <v>14673</v>
+      </c>
+      <c r="N56" s="0" t="n">
+        <v>13873</v>
+      </c>
+      <c r="O56" s="0" t="n">
+        <v>13198</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G57" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="1" t="n">
+        <v>275037</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>143695</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>72993</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>37523</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>26386</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <v>28972</v>
+      </c>
+      <c r="N57" s="0" t="n">
+        <v>27142</v>
+      </c>
+      <c r="O57" s="0" t="n">
+        <v>26677</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <v>565296</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>296328</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>147240</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>76607</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>65983</v>
+      </c>
+      <c r="M58" s="0" t="n">
+        <v>59934</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>56197</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <v>52981</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2749,7 +3567,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2775,7 +3593,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>